<commit_message>
quase terminando o primeiro artigo
</commit_message>
<xml_diff>
--- a/listas.xlsx
+++ b/listas.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saull\OneDrive\Documentos\GitHub\Dados-publicos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C178FFE-8A68-4C04-884B-D4EEFAEF105F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDDFCE5-BF3F-40F5-BD0E-408E7423AFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{A8E08153-F332-4DCB-98E1-F5E2C0132F7D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A8E08153-F332-4DCB-98E1-F5E2C0132F7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="14">
   <si>
     <t>INDEX</t>
   </si>
@@ -73,6 +74,9 @@
   <si>
     <t>name_list</t>
   </si>
+  <si>
+    <t>name_list.append(df_dep_info['nome'][count-1])</t>
+  </si>
 </sst>
 </file>
 
@@ -80,9 +84,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +114,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -131,7 +140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -290,12 +299,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -327,50 +345,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -687,94 +729,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98673E85-838C-4C29-AA0E-F46A51583CC6}">
-  <dimension ref="B1:T19"/>
+  <dimension ref="F4:T19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5:O19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="17">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>100</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6">
-        <v>101</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="14" t="s">
+    <row r="4" spans="6:20" ht="15.75" thickBot="1"/>
+    <row r="5" spans="6:20" ht="19.5" thickBot="1">
+      <c r="F5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16"/>
-      <c r="K5" s="11" t="s">
+      <c r="G5" s="25"/>
+      <c r="H5" s="26"/>
+      <c r="K5" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="12"/>
-      <c r="N5" s="11" t="s">
+      <c r="L5" s="28"/>
+      <c r="N5" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="12"/>
-      <c r="Q5" s="14" t="s">
+      <c r="O5" s="28"/>
+      <c r="Q5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="16"/>
-    </row>
-    <row r="6" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="6">
-        <v>102</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="26"/>
+    </row>
+    <row r="6" spans="6:20" ht="15.75" thickBot="1">
       <c r="F6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="16" t="s">
         <v>2</v>
       </c>
       <c r="H6" s="9" t="s">
@@ -805,32 +800,23 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="6">
-        <v>103</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
-      </c>
+    <row r="7" spans="6:20">
       <c r="F7" s="5">
         <v>0</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="17">
         <v>100</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="13">
         <v>1</v>
       </c>
-      <c r="K7" s="17">
+      <c r="K7" s="11">
         <v>0</v>
       </c>
       <c r="L7" s="5">
         <v>100</v>
       </c>
-      <c r="N7" s="17">
+      <c r="N7" s="11">
         <v>0</v>
       </c>
       <c r="O7" s="5" t="s">
@@ -845,27 +831,18 @@
       <c r="S7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="T7" s="19">
+      <c r="T7" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>11</v>
-      </c>
+    <row r="8" spans="6:20">
       <c r="F8" s="6">
         <v>1</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="18">
         <v>100</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="14">
         <v>2</v>
       </c>
       <c r="K8" s="1">
@@ -889,18 +866,18 @@
       <c r="S8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="T8" s="20">
+      <c r="T8" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="6:20">
       <c r="F9" s="6">
         <v>2</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="18">
         <v>100</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="14">
         <v>3</v>
       </c>
       <c r="K9" s="1">
@@ -924,18 +901,18 @@
       <c r="S9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="T9" s="20">
+      <c r="T9" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="6:20">
       <c r="F10" s="6">
         <v>3</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="18">
         <v>102</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="14">
         <v>4</v>
       </c>
       <c r="K10" s="1">
@@ -959,18 +936,18 @@
       <c r="S10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="T10" s="20">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="T10" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="6:20">
       <c r="F11" s="6">
         <v>4</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="18">
         <v>102</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="14">
         <v>5</v>
       </c>
       <c r="K11" s="1">
@@ -994,18 +971,18 @@
       <c r="S11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="T11" s="20">
+      <c r="T11" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="6:20">
       <c r="F12" s="6">
         <v>5</v>
       </c>
-      <c r="G12" s="24">
-        <v>103</v>
-      </c>
-      <c r="H12" s="20">
+      <c r="G12" s="18">
+        <v>103</v>
+      </c>
+      <c r="H12" s="14">
         <v>6</v>
       </c>
       <c r="K12" s="1">
@@ -1029,18 +1006,18 @@
       <c r="S12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="T12" s="20">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="T12" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="6:20">
       <c r="F13" s="6">
         <v>6</v>
       </c>
-      <c r="G13" s="24">
-        <v>103</v>
-      </c>
-      <c r="H13" s="20">
+      <c r="G13" s="18">
+        <v>103</v>
+      </c>
+      <c r="H13" s="14">
         <v>7</v>
       </c>
       <c r="K13" s="1">
@@ -1064,18 +1041,18 @@
       <c r="S13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="T13" s="20">
+      <c r="T13" s="14">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="6:20">
       <c r="F14" s="6">
         <v>7</v>
       </c>
-      <c r="G14" s="24">
-        <v>103</v>
-      </c>
-      <c r="H14" s="20">
+      <c r="G14" s="18">
+        <v>103</v>
+      </c>
+      <c r="H14" s="14">
         <v>8</v>
       </c>
       <c r="K14" s="1">
@@ -1099,18 +1076,18 @@
       <c r="S14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="T14" s="20">
+      <c r="T14" s="14">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="6:20">
       <c r="F15" s="6">
         <v>8</v>
       </c>
-      <c r="G15" s="24">
-        <v>103</v>
-      </c>
-      <c r="H15" s="20">
+      <c r="G15" s="18">
+        <v>103</v>
+      </c>
+      <c r="H15" s="14">
         <v>9</v>
       </c>
       <c r="K15" s="1">
@@ -1134,18 +1111,18 @@
       <c r="S15" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="T15" s="20">
+      <c r="T15" s="14">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="6:20">
       <c r="F16" s="6">
         <v>9</v>
       </c>
-      <c r="G16" s="24">
-        <v>103</v>
-      </c>
-      <c r="H16" s="20">
+      <c r="G16" s="18">
+        <v>103</v>
+      </c>
+      <c r="H16" s="14">
         <v>10</v>
       </c>
       <c r="K16" s="1">
@@ -1169,18 +1146,18 @@
       <c r="S16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="T16" s="20">
+      <c r="T16" s="14">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="6:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:20">
       <c r="F17" s="6">
         <v>10</v>
       </c>
-      <c r="G17" s="24">
-        <v>103</v>
-      </c>
-      <c r="H17" s="20">
+      <c r="G17" s="18">
+        <v>103</v>
+      </c>
+      <c r="H17" s="14">
         <v>11</v>
       </c>
       <c r="K17" s="1">
@@ -1204,18 +1181,18 @@
       <c r="S17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="T17" s="20">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="6:20" x14ac:dyDescent="0.3">
+      <c r="T17" s="14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="6:20">
       <c r="F18" s="6">
         <v>11</v>
       </c>
-      <c r="G18" s="24">
-        <v>103</v>
-      </c>
-      <c r="H18" s="20">
+      <c r="G18" s="18">
+        <v>103</v>
+      </c>
+      <c r="H18" s="14">
         <v>12</v>
       </c>
       <c r="K18" s="1">
@@ -1239,18 +1216,18 @@
       <c r="S18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="T18" s="20">
+      <c r="T18" s="14">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="6:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:20" ht="15.75" thickBot="1">
       <c r="F19" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="21" t="s">
+      <c r="G19" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="15" t="s">
         <v>11</v>
       </c>
       <c r="K19" s="3" t="s">
@@ -1274,13 +1251,12 @@
       <c r="S19" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="T19" s="21" t="s">
+      <c r="T19" s="15" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B2:D2"/>
+  <mergeCells count="4">
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="N5:O5"/>
@@ -1289,4 +1265,567 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE32E5EA-21FC-4378-8FFC-2A29293FFFFC}">
+  <dimension ref="B2:T33"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:20" ht="19.5" thickBot="1">
+      <c r="I2" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+    </row>
+    <row r="3" spans="2:20" ht="15.75" thickBot="1">
+      <c r="I3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20">
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="21">
+        <v>100</v>
+      </c>
+      <c r="K4" s="13">
+        <v>1</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20">
+      <c r="I5" s="6">
+        <v>1</v>
+      </c>
+      <c r="J5" s="22">
+        <v>100</v>
+      </c>
+      <c r="K5" s="14">
+        <v>2</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20">
+      <c r="I6" s="6">
+        <v>2</v>
+      </c>
+      <c r="J6" s="22">
+        <v>100</v>
+      </c>
+      <c r="K6" s="14">
+        <v>3</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20">
+      <c r="I7" s="6">
+        <v>3</v>
+      </c>
+      <c r="J7" s="22">
+        <v>102</v>
+      </c>
+      <c r="K7" s="14">
+        <v>4</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20">
+      <c r="I8" s="6">
+        <v>4</v>
+      </c>
+      <c r="J8" s="22">
+        <v>102</v>
+      </c>
+      <c r="K8" s="14">
+        <v>5</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20">
+      <c r="I9" s="6">
+        <v>5</v>
+      </c>
+      <c r="J9" s="22">
+        <v>103</v>
+      </c>
+      <c r="K9" s="14">
+        <v>6</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20">
+      <c r="I10" s="6">
+        <v>6</v>
+      </c>
+      <c r="J10" s="22">
+        <v>103</v>
+      </c>
+      <c r="K10" s="14">
+        <v>7</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20">
+      <c r="I11" s="6">
+        <v>7</v>
+      </c>
+      <c r="J11" s="22">
+        <v>103</v>
+      </c>
+      <c r="K11" s="14">
+        <v>8</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" ht="19.5" thickBot="1">
+      <c r="B12" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="I12" s="6">
+        <v>8</v>
+      </c>
+      <c r="J12" s="22">
+        <v>103</v>
+      </c>
+      <c r="K12" s="14">
+        <v>9</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" ht="15.75" thickBot="1">
+      <c r="B13" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="6">
+        <v>9</v>
+      </c>
+      <c r="J13" s="22">
+        <v>103</v>
+      </c>
+      <c r="K13" s="14">
+        <v>10</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20">
+      <c r="B14" s="11">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5">
+        <v>100</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="6">
+        <v>10</v>
+      </c>
+      <c r="J14" s="22">
+        <v>103</v>
+      </c>
+      <c r="K14" s="14">
+        <v>11</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="T14" s="33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20">
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="6">
+        <v>101</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="6">
+        <v>11</v>
+      </c>
+      <c r="J15" s="22">
+        <v>103</v>
+      </c>
+      <c r="K15" s="14">
+        <v>12</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" ht="15.75" thickBot="1">
+      <c r="B16" s="1">
+        <v>2</v>
+      </c>
+      <c r="C16" s="6">
+        <v>102</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
+      <c r="B17" s="1">
+        <v>3</v>
+      </c>
+      <c r="C17" s="6">
+        <v>103</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="15.75" thickBot="1">
+      <c r="B18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="19.5" thickBot="1">
+      <c r="I19" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="28"/>
+      <c r="L19" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="M19" s="28"/>
+    </row>
+    <row r="20" spans="2:13" ht="15.75" thickBot="1">
+      <c r="I20" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13">
+      <c r="I21" s="11">
+        <v>0</v>
+      </c>
+      <c r="J21" s="5">
+        <v>100</v>
+      </c>
+      <c r="L21" s="11">
+        <v>0</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13">
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
+      <c r="J22" s="6">
+        <v>100</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13">
+      <c r="I23" s="1">
+        <v>2</v>
+      </c>
+      <c r="J23" s="6">
+        <v>100</v>
+      </c>
+      <c r="L23" s="1">
+        <v>2</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13">
+      <c r="I24" s="1">
+        <v>3</v>
+      </c>
+      <c r="J24" s="6">
+        <v>102</v>
+      </c>
+      <c r="L24" s="1">
+        <v>3</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13">
+      <c r="I25" s="1">
+        <v>4</v>
+      </c>
+      <c r="J25" s="6">
+        <v>102</v>
+      </c>
+      <c r="L25" s="1">
+        <v>4</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13">
+      <c r="I26" s="1">
+        <v>5</v>
+      </c>
+      <c r="J26" s="6">
+        <v>103</v>
+      </c>
+      <c r="L26" s="1">
+        <v>5</v>
+      </c>
+      <c r="M26" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13">
+      <c r="I27" s="1">
+        <v>6</v>
+      </c>
+      <c r="J27" s="6">
+        <v>103</v>
+      </c>
+      <c r="L27" s="1">
+        <v>6</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13">
+      <c r="I28" s="1">
+        <v>7</v>
+      </c>
+      <c r="J28" s="6">
+        <v>103</v>
+      </c>
+      <c r="L28" s="1">
+        <v>7</v>
+      </c>
+      <c r="M28" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13">
+      <c r="I29" s="1">
+        <v>8</v>
+      </c>
+      <c r="J29" s="6">
+        <v>103</v>
+      </c>
+      <c r="L29" s="1">
+        <v>8</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13">
+      <c r="I30" s="1">
+        <v>9</v>
+      </c>
+      <c r="J30" s="6">
+        <v>103</v>
+      </c>
+      <c r="L30" s="1">
+        <v>9</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13">
+      <c r="I31" s="1">
+        <v>10</v>
+      </c>
+      <c r="J31" s="6">
+        <v>103</v>
+      </c>
+      <c r="L31" s="1">
+        <v>10</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13">
+      <c r="I32" s="1">
+        <v>11</v>
+      </c>
+      <c r="J32" s="6">
+        <v>103</v>
+      </c>
+      <c r="L32" s="1">
+        <v>11</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="9:13" ht="15.75" thickBot="1">
+      <c r="I33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="I2:M2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>